<commit_message>
a few updates like color
</commit_message>
<xml_diff>
--- a/input_case.xlsx
+++ b/input_case.xlsx
@@ -714,7 +714,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -744,6 +744,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -843,14 +847,14 @@
   <dimension ref="A1:BP7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.71"/>
@@ -897,7 +901,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="0" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="0" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="0" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="0" width="15.71"/>
@@ -1104,499 +1108,499 @@
       <c r="BM1" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="BN1" s="0" t="s">
+      <c r="BN1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="BO1" s="0" t="s">
+      <c r="BO1" s="8" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" s="8" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+    <row r="2" s="9" customFormat="true" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="8" t="s">
+      <c r="L2" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="8" t="s">
+      <c r="R2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="T2" s="8" t="s">
+      <c r="T2" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AC2" s="8" t="s">
+      <c r="AC2" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AD2" s="8" t="s">
+      <c r="AD2" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AE2" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AF2" s="8" t="s">
+      <c r="AF2" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AG2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" s="8" t="s">
+      <c r="AH2" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AI2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AK2" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AL2" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AM2" s="8" t="s">
+      <c r="AM2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AN2" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AO2" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AS2" s="8" t="s">
+      <c r="AS2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AV2" s="8" t="s">
+      <c r="AV2" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="AW2" s="8" t="s">
+      <c r="AW2" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AX2" s="8" t="s">
+      <c r="AX2" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AY2" s="8" t="s">
+      <c r="AY2" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="AZ2" s="8" t="s">
+      <c r="AZ2" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="BA2" s="8" t="s">
+      <c r="BA2" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="BD2" s="8" t="s">
+      <c r="BD2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="BE2" s="8" t="s">
+      <c r="BE2" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="BG2" s="8" t="s">
+      <c r="BG2" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="BH2" s="8" t="s">
+      <c r="BH2" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BI2" s="8" t="s">
+      <c r="BI2" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BJ2" s="8" t="s">
+      <c r="BJ2" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="BK2" s="8" t="s">
+      <c r="BK2" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="BL2" s="8" t="s">
+      <c r="BL2" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="BM2" s="9" t="s">
+      <c r="BM2" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+    <row r="3" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="V3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Y3" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="Z3" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="AA3" s="8" t="s">
+      <c r="AA3" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="AB3" s="8" t="s">
+      <c r="AB3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AC3" s="8" t="s">
+      <c r="AC3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="AD3" s="8" t="s">
+      <c r="AD3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AE3" s="8" t="s">
+      <c r="AE3" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AF3" s="8" t="s">
+      <c r="AF3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AG3" s="8" t="s">
+      <c r="AG3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AH3" s="8" t="s">
+      <c r="AH3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AI3" s="8" t="s">
+      <c r="AI3" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AJ3" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="AK3" s="8" t="s">
+      <c r="AK3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AL3" s="8" t="s">
+      <c r="AL3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AM3" s="8" t="s">
+      <c r="AM3" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="AN3" s="8" t="s">
+      <c r="AN3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="AO3" s="8" t="s">
+      <c r="AO3" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="AP3" s="8" t="s">
+      <c r="AP3" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="AQ3" s="8" t="s">
+      <c r="AQ3" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="AS3" s="8" t="s">
+      <c r="AS3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="AT3" s="8" t="s">
+      <c r="AT3" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="AU3" s="8" t="s">
+      <c r="AU3" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="AV3" s="8" t="s">
+      <c r="AV3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="AW3" s="8" t="s">
+      <c r="AW3" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="AX3" s="8" t="s">
+      <c r="AX3" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="AY3" s="8" t="s">
+      <c r="AY3" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="AZ3" s="8" t="s">
+      <c r="AZ3" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="BA3" s="8" t="s">
+      <c r="BA3" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="BB3" s="8" t="s">
+      <c r="BB3" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="BC3" s="8" t="s">
+      <c r="BC3" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="BD3" s="8" t="s">
+      <c r="BD3" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="BE3" s="8" t="s">
+      <c r="BE3" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="BG3" s="8" t="s">
+      <c r="BG3" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="BH3" s="8" t="s">
+      <c r="BH3" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BI3" s="8" t="s">
+      <c r="BI3" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BJ3" s="8" t="s">
+      <c r="BJ3" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="BK3" s="8" t="s">
+      <c r="BK3" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="BL3" s="8" t="s">
+      <c r="BL3" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="BM3" s="9" t="s">
+      <c r="BM3" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="BN3" s="8" t="s">
+      <c r="BN3" s="9" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="4" s="8" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+    <row r="4" s="9" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="I4" s="8" t="s">
+      <c r="I4" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="K4" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="O4" s="8" t="s">
+      <c r="O4" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="Q4" s="8" t="s">
+      <c r="Q4" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="S4" s="8" t="s">
+      <c r="S4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="T4" s="8" t="s">
+      <c r="T4" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="U4" s="8" t="s">
+      <c r="U4" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="V4" s="8" t="s">
+      <c r="V4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="W4" s="8" t="s">
+      <c r="W4" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="AB4" s="8" t="s">
+      <c r="AB4" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AC4" s="8" t="s">
+      <c r="AC4" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="AE4" s="8" t="s">
+      <c r="AE4" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AF4" s="8" t="s">
+      <c r="AF4" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AG4" s="8" t="s">
+      <c r="AG4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AH4" s="8" t="s">
+      <c r="AH4" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AI4" s="8" t="s">
+      <c r="AI4" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AJ4" s="8" t="s">
+      <c r="AJ4" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="AK4" s="8" t="s">
+      <c r="AK4" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AL4" s="8" t="s">
+      <c r="AL4" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AM4" s="8" t="s">
+      <c r="AM4" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AN4" s="8" t="s">
+      <c r="AN4" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="AT4" s="8" t="s">
+      <c r="AT4" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="AU4" s="8" t="s">
+      <c r="AU4" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="AW4" s="8" t="s">
+      <c r="AW4" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="BA4" s="8" t="s">
+      <c r="BA4" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="BC4" s="8" t="s">
+      <c r="BC4" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="BD4" s="8" t="s">
+      <c r="BD4" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="BE4" s="8" t="s">
+      <c r="BE4" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="BG4" s="8" t="s">
+      <c r="BG4" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="BH4" s="8" t="s">
+      <c r="BH4" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BI4" s="8" t="s">
+      <c r="BI4" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BJ4" s="8" t="s">
+      <c r="BJ4" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="BK4" s="8" t="s">
+      <c r="BK4" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="BL4" s="8" t="s">
+      <c r="BL4" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="BM4" s="9" t="s">
+      <c r="BM4" s="10" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1712,176 +1716,176 @@
         <v>160</v>
       </c>
     </row>
-    <row r="7" s="8" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+    <row r="7" s="9" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="K7" s="8" t="s">
+      <c r="K7" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="M7" s="8" t="s">
+      <c r="M7" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="P7" s="8" t="s">
+      <c r="P7" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="Q7" s="8" t="s">
+      <c r="Q7" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="R7" s="8" t="s">
+      <c r="R7" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="T7" s="8" t="s">
+      <c r="T7" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="U7" s="8" t="s">
+      <c r="U7" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="V7" s="8" t="s">
+      <c r="V7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="X7" s="8" t="s">
+      <c r="X7" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="Y7" s="8" t="s">
+      <c r="Y7" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="Z7" s="8" t="s">
+      <c r="Z7" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="AA7" s="8" t="s">
+      <c r="AA7" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="AB7" s="8" t="s">
+      <c r="AB7" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="AC7" s="8" t="s">
+      <c r="AC7" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="AD7" s="8" t="s">
+      <c r="AD7" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="AE7" s="8" t="s">
+      <c r="AE7" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="AF7" s="8" t="s">
+      <c r="AF7" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="AG7" s="8" t="s">
+      <c r="AG7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AH7" s="8" t="s">
+      <c r="AH7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="AI7" s="8" t="s">
+      <c r="AI7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="AJ7" s="8" t="s">
+      <c r="AJ7" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="AK7" s="8" t="s">
+      <c r="AK7" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AL7" s="8" t="s">
+      <c r="AL7" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="AM7" s="8" t="s">
+      <c r="AM7" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="AN7" s="8" t="s">
+      <c r="AN7" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="AO7" s="8" t="s">
+      <c r="AO7" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="AP7" s="8" t="s">
+      <c r="AP7" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="AR7" s="8" t="s">
+      <c r="AR7" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="AT7" s="8" t="s">
+      <c r="AT7" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="AU7" s="8" t="s">
+      <c r="AU7" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="AY7" s="8" t="s">
+      <c r="AY7" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="AZ7" s="8" t="s">
+      <c r="AZ7" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="BA7" s="8" t="s">
+      <c r="BA7" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="BB7" s="8" t="s">
+      <c r="BB7" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="BC7" s="8" t="s">
+      <c r="BC7" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="BD7" s="8" t="s">
+      <c r="BD7" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="BE7" s="8" t="s">
+      <c r="BE7" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="BG7" s="8" t="s">
+      <c r="BG7" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="BH7" s="8" t="s">
+      <c r="BH7" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="BI7" s="8" t="s">
+      <c r="BI7" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="BJ7" s="8" t="s">
+      <c r="BJ7" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="BK7" s="8" t="s">
+      <c r="BK7" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="BL7" s="8" t="s">
+      <c r="BL7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="BM7" s="9" t="s">
+      <c r="BM7" s="10" t="s">
         <v>183</v>
       </c>
     </row>

</xml_diff>